<commit_message>
Database Updated, Prioritise Script Corrected, Debug Data updated.
</commit_message>
<xml_diff>
--- a/Score_Manager.xlsx
+++ b/Score_Manager.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77167DC3-2303-4059-83FC-8C2606FE4B17}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBB0C38-9212-4EC4-B887-633379F6FBC4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>Graphics</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Solid State Drive</t>
+  </si>
+  <si>
+    <t>CPU</t>
   </si>
 </sst>
 </file>
@@ -230,6 +233,33 @@
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -237,33 +267,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -549,7 +552,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,253 +576,259 @@
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="2" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="2" t="s">
+      <c r="H1" s="12"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="2" t="s">
+      <c r="K1" s="12"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="4"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="13"/>
     </row>
     <row r="2" spans="1:15" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="8">
         <v>9</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="2">
         <v>10</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="2">
         <v>10</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="2">
         <v>3</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="2">
         <v>5</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="7" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="2">
         <v>8</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="2">
         <v>8</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="2">
         <v>2</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="2">
         <v>6</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="7" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="2">
         <v>5</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="2">
         <v>6</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="2">
         <v>1</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="M4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="2">
         <v>7</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="7" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="2">
         <v>3</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="8" t="s">
+      <c r="G5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="2">
+        <v>5</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="2">
         <v>2</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="8"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="6"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:15" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="7" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="2">
         <v>9</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="6"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="3"/>
     </row>
     <row r="7" spans="1:15" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="7" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="2">
         <v>7</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="6"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="3"/>
     </row>
     <row r="8" spans="1:15" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="9" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="2">
         <v>4</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="6"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="3"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>

</xml_diff>